<commit_message>
update pinmap with pullup todo
</commit_message>
<xml_diff>
--- a/pinmap.xlsx
+++ b/pinmap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -165,9 +165,6 @@
     <t>VPSI_HD</t>
   </si>
   <si>
-    <t>PSRAM_CS</t>
-  </si>
-  <si>
     <t>PSRAM_CLK</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>BOARD_INT_SPI_MOSI</t>
   </si>
   <si>
-    <t>LCD_PIN_CS</t>
-  </si>
-  <si>
     <t>FLASH, PSRAM_SIO[3]</t>
   </si>
   <si>
@@ -219,9 +213,6 @@
     <t>LCD_PIN_DC</t>
   </si>
   <si>
-    <t>TOUCH_PIN_CS</t>
-  </si>
-  <si>
     <t>LCD pins done</t>
   </si>
   <si>
@@ -243,9 +234,6 @@
     <t>HSPI_HD (boot:pulldwn)</t>
   </si>
   <si>
-    <t>SD_CS</t>
-  </si>
-  <si>
     <t>SD pins done</t>
   </si>
   <si>
@@ -279,13 +267,34 @@
     <t>UART pins done</t>
   </si>
   <si>
-    <t>IO (MCP23S17)</t>
-  </si>
-  <si>
-    <t>IO_CS</t>
-  </si>
-  <si>
     <t>IO_IRQ</t>
+  </si>
+  <si>
+    <t>IO (MCP23S17) done</t>
+  </si>
+  <si>
+    <t>ANALOG done</t>
+  </si>
+  <si>
+    <t>ANALOG_LEFT (ADC1_CH4 (GPIO 32))</t>
+  </si>
+  <si>
+    <t>ANALOG_RIGHT (ADC1_CH5 (GPIO 33))</t>
+  </si>
+  <si>
+    <t>PSRAM_CS (add pullup?)</t>
+  </si>
+  <si>
+    <t>SD_CS (use pullup?)</t>
+  </si>
+  <si>
+    <t>IO_CS (use pullup?)</t>
+  </si>
+  <si>
+    <t>TOUCH_PIN_CS (use internal pullup after boot?)</t>
+  </si>
+  <si>
+    <t>LCD_PIN_CS (use internal pullup after boot?)</t>
   </si>
 </sst>
 </file>
@@ -347,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -363,6 +372,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -664,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +761,7 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -764,7 +776,7 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -779,7 +791,7 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -794,7 +806,7 @@
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -809,7 +821,7 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -823,8 +835,8 @@
         <v>36</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="4" t="s">
-        <v>88</v>
+      <c r="E10" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -853,7 +865,9 @@
         <v>36</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -866,7 +880,9 @@
         <v>36</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -882,12 +898,12 @@
         <v>38</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="6">
         <v>14</v>
@@ -899,7 +915,7 @@
         <v>40</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -929,7 +945,7 @@
         <v>41</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -946,7 +962,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,7 +979,7 @@
         <v>39</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -980,7 +996,7 @@
         <v>39</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -997,7 +1013,7 @@
         <v>39</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1014,7 +1030,7 @@
         <v>39</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1031,12 +1047,12 @@
         <v>39</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="6">
         <v>23</v>
@@ -1045,15 +1061,15 @@
         <v>36</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="6">
         <v>24</v>
@@ -1062,15 +1078,15 @@
         <v>36</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="6">
         <v>25</v>
@@ -1079,15 +1095,15 @@
         <v>36</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B27" s="6">
         <v>26</v>
@@ -1096,10 +1112,10 @@
         <v>36</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1114,7 +1130,7 @@
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="4" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1129,12 +1145,12 @@
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="6">
         <v>29</v>
@@ -1215,7 +1231,7 @@
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1230,7 +1246,7 @@
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1278,47 +1294,52 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D41" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D42" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D43" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D44" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D45" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D46" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D47" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D48" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>